<commit_message>
Updated geolocker and firefox paths. Added automatic lib update
</commit_message>
<xml_diff>
--- a/wyniki_ofert_z_filtra.xlsx
+++ b/wyniki_ofert_z_filtra.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -552,7 +552,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -591,7 +591,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -630,7 +630,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -669,7 +669,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -708,7 +708,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -786,7 +786,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -825,7 +825,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -864,7 +864,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -903,7 +903,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -942,7 +942,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -981,7 +981,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1098,7 +1098,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1332,7 +1332,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1410,7 +1410,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1605,7 +1605,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1644,7 +1644,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -1800,7 +1800,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -1839,7 +1839,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -1878,7 +1878,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -1917,7 +1917,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -2034,7 +2034,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -2112,7 +2112,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -2307,7 +2307,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -2424,7 +2424,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -2463,7 +2463,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -2502,7 +2502,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F54" t="n">
@@ -2580,7 +2580,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F57" t="n">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F58" t="n">
@@ -2736,7 +2736,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F59" t="n">
@@ -2775,7 +2775,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F60" t="n">
@@ -2814,7 +2814,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F61" t="n">
@@ -2853,7 +2853,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F62" t="n">
@@ -2970,7 +2970,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F65" t="n">
@@ -3009,7 +3009,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F66" t="n">
@@ -3087,7 +3087,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F68" t="n">
@@ -3126,7 +3126,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F69" t="n">
@@ -3165,7 +3165,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F70" t="n">
@@ -3204,7 +3204,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F71" t="n">
@@ -3477,7 +3477,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F78" t="n">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F82" t="n">
@@ -3672,7 +3672,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F83" t="n">
@@ -3711,7 +3711,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F84" t="n">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F85" t="n">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F86" t="n">
@@ -3828,7 +3828,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F87" t="n">
@@ -3867,7 +3867,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F88" t="n">
@@ -3906,7 +3906,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F89" t="n">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F90" t="n">
@@ -3984,7 +3984,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F91" t="n">
@@ -4023,7 +4023,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F92" t="n">
@@ -4062,7 +4062,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F93" t="n">
@@ -4101,7 +4101,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F94" t="n">
@@ -4140,7 +4140,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F95" t="n">
@@ -4179,7 +4179,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F96" t="n">
@@ -4218,7 +4218,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F97" t="n">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F98" t="n">
@@ -4296,7 +4296,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F99" t="n">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F100" t="n">
@@ -4374,7 +4374,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F101" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F102" t="n">
@@ -4491,7 +4491,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F104" t="n">
@@ -4530,7 +4530,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F105" t="n">
@@ -4569,7 +4569,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F106" t="n">
@@ -4608,7 +4608,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F107" t="n">
@@ -4724,7 +4724,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -4763,7 +4763,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -4802,7 +4802,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -4841,7 +4841,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -4880,7 +4880,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -4919,7 +4919,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -4958,7 +4958,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -4997,7 +4997,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -5153,7 +5153,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -5309,7 +5309,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -5543,7 +5543,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -5582,7 +5582,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -5660,7 +5660,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -5777,7 +5777,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -5816,7 +5816,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -5855,7 +5855,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -5894,7 +5894,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -5933,7 +5933,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -5972,7 +5972,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -6011,7 +6011,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -6050,7 +6050,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -6089,7 +6089,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -6128,7 +6128,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -6167,7 +6167,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -6206,7 +6206,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -6284,7 +6284,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -6323,7 +6323,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -6362,7 +6362,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -6440,7 +6440,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -6479,7 +6479,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -6518,7 +6518,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -6557,7 +6557,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -6596,7 +6596,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -6635,7 +6635,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -6674,7 +6674,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -6752,7 +6752,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F54" t="n">
@@ -6830,7 +6830,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F56" t="n">
@@ -6869,7 +6869,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F57" t="n">
@@ -7064,7 +7064,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F62" t="n">
@@ -7103,7 +7103,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F63" t="n">
@@ -7142,7 +7142,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F64" t="n">
@@ -7181,7 +7181,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F65" t="n">
@@ -7220,7 +7220,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F66" t="n">
@@ -7298,7 +7298,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F68" t="n">
@@ -7337,7 +7337,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F69" t="n">
@@ -7376,7 +7376,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F70" t="n">
@@ -7415,7 +7415,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F71" t="n">
@@ -7454,7 +7454,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F72" t="n">
@@ -7493,7 +7493,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F73" t="n">
@@ -7532,7 +7532,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F74" t="n">
@@ -7571,7 +7571,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F75" t="n">
@@ -7649,7 +7649,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>2025-07-22</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="F77" t="n">

</xml_diff>

<commit_message>
Automatyczna aktualizacja Excela [2025-07-27 06:26:26]
</commit_message>
<xml_diff>
--- a/wyniki_ofert_z_filtra.xlsx
+++ b/wyniki_ofert_z_filtra.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -552,7 +552,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -591,7 +591,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -630,7 +630,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -679,7 +679,7 @@
         <v>13.95</v>
       </c>
       <c r="H6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -708,7 +708,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -786,7 +786,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -825,7 +825,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -864,7 +864,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -903,7 +903,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -952,7 +952,7 @@
         <v>27.57</v>
       </c>
       <c r="H13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -981,7 +981,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1098,7 +1098,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1332,7 +1332,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1410,7 +1410,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1605,7 +1605,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1644,7 +1644,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -1800,7 +1800,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -1849,7 +1849,7 @@
         <v>30.52</v>
       </c>
       <c r="H36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
@@ -1878,7 +1878,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -1917,7 +1917,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -2034,7 +2034,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -2112,7 +2112,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -2307,7 +2307,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -2424,7 +2424,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -2463,7 +2463,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -2502,7 +2502,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F54" t="n">
@@ -2580,7 +2580,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F57" t="n">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F58" t="n">
@@ -2736,7 +2736,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F59" t="n">
@@ -2775,7 +2775,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F60" t="n">
@@ -2814,7 +2814,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F61" t="n">
@@ -2853,7 +2853,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F62" t="n">
@@ -2980,7 +2980,7 @@
         <v>251.83</v>
       </c>
       <c r="H65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65" t="inlineStr">
         <is>
@@ -3019,7 +3019,7 @@
         <v>27.23</v>
       </c>
       <c r="H66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I66" t="inlineStr">
         <is>
@@ -3097,7 +3097,7 @@
         <v>22.5</v>
       </c>
       <c r="H68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I68" t="inlineStr">
         <is>
@@ -3487,7 +3487,7 @@
         <v>22.16</v>
       </c>
       <c r="H78" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I78" t="inlineStr">
         <is>
@@ -3643,7 +3643,7 @@
         <v>25.92</v>
       </c>
       <c r="H82" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I82" t="inlineStr">
         <is>
@@ -3672,7 +3672,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F83" t="n">
@@ -3711,7 +3711,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F84" t="n">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F85" t="n">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F86" t="n">
@@ -3828,7 +3828,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F87" t="n">
@@ -3867,7 +3867,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F88" t="n">
@@ -3906,7 +3906,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F89" t="n">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F90" t="n">
@@ -3984,7 +3984,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F91" t="n">
@@ -4023,7 +4023,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F92" t="n">
@@ -4062,7 +4062,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F93" t="n">
@@ -4101,7 +4101,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F94" t="n">
@@ -4150,7 +4150,7 @@
         <v>14.32</v>
       </c>
       <c r="H95" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I95" t="inlineStr">
         <is>
@@ -4179,7 +4179,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F96" t="n">
@@ -4218,7 +4218,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F97" t="n">
@@ -4267,7 +4267,7 @@
         <v>20.79</v>
       </c>
       <c r="H98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I98" t="inlineStr">
         <is>
@@ -4306,7 +4306,7 @@
         <v>33.81</v>
       </c>
       <c r="H99" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I99" t="inlineStr">
         <is>
@@ -4345,7 +4345,7 @@
         <v>33.81</v>
       </c>
       <c r="H100" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I100" t="inlineStr">
         <is>
@@ -4384,7 +4384,7 @@
         <v>33.81</v>
       </c>
       <c r="H101" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I101" t="inlineStr">
         <is>
@@ -4423,7 +4423,7 @@
         <v>33.81</v>
       </c>
       <c r="H102" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I102" t="inlineStr">
         <is>
@@ -4462,7 +4462,7 @@
         <v>33.81</v>
       </c>
       <c r="H103" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I103" t="inlineStr">
         <is>
@@ -4501,7 +4501,7 @@
         <v>22.02</v>
       </c>
       <c r="H104" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I104" t="inlineStr">
         <is>
@@ -4540,7 +4540,7 @@
         <v>39.89</v>
       </c>
       <c r="H105" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I105" t="inlineStr">
         <is>
@@ -4579,7 +4579,7 @@
         <v>33.81</v>
       </c>
       <c r="H106" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I106" t="inlineStr">
         <is>
@@ -4618,7 +4618,7 @@
         <v>10.54</v>
       </c>
       <c r="H107" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I107" t="inlineStr">
         <is>
@@ -4657,7 +4657,7 @@
         <v>23.8</v>
       </c>
       <c r="H108" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I108" t="inlineStr">
         <is>
@@ -4696,7 +4696,7 @@
         <v>20.79</v>
       </c>
       <c r="H109" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I109" t="inlineStr">
         <is>
@@ -4735,7 +4735,7 @@
         <v>26.66</v>
       </c>
       <c r="H110" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I110" t="inlineStr">
         <is>
@@ -4754,7 +4754,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4841,7 +4841,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -4880,7 +4880,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -4919,7 +4919,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -4958,7 +4958,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -4997,7 +4997,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -5036,7 +5036,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -5075,7 +5075,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -5114,7 +5114,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -5270,7 +5270,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -5426,7 +5426,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -5660,7 +5660,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -5699,7 +5699,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -5777,7 +5777,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -5894,7 +5894,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -5933,7 +5933,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -5982,7 +5982,7 @@
         <v>32.19</v>
       </c>
       <c r="H31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
@@ -6050,7 +6050,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -6089,7 +6089,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -6128,7 +6128,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -6167,7 +6167,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -6206,7 +6206,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -6245,7 +6245,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -6284,7 +6284,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -6323,7 +6323,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -6401,7 +6401,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -6440,7 +6440,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -6479,7 +6479,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -6557,7 +6557,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -6596,7 +6596,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -6635,7 +6635,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -6674,7 +6674,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -6713,7 +6713,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -6752,7 +6752,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -6791,7 +6791,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -6957,7 +6957,7 @@
         <v>24.58</v>
       </c>
       <c r="H56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" t="inlineStr">
         <is>
@@ -7181,7 +7181,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F62" t="n">
@@ -7220,7 +7220,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F63" t="n">
@@ -7298,7 +7298,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F65" t="n">
@@ -7337,7 +7337,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F66" t="n">
@@ -7415,7 +7415,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F68" t="n">
@@ -7454,7 +7454,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F69" t="n">
@@ -7493,7 +7493,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F70" t="n">
@@ -7532,7 +7532,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F71" t="n">
@@ -7571,7 +7571,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F72" t="n">
@@ -7610,7 +7610,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F73" t="n">
@@ -7649,7 +7649,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F74" t="n">
@@ -7688,7 +7688,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F75" t="n">
@@ -7776,7 +7776,7 @@
         <v>35.8</v>
       </c>
       <c r="H77" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I77" t="inlineStr">
         <is>
@@ -7805,7 +7805,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F78" t="n">
@@ -7844,7 +7844,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="F79" t="n">
@@ -7893,11 +7893,206 @@
         <v>26.66</v>
       </c>
       <c r="H80" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I80" t="inlineStr">
         <is>
           <t>https://www.otodom.pl/hpr/pl/oferta/dzialki-budowlane-w-zabierzowie-bochenskim-ID4xotB</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Działka Budowlana | 16 ar | Jawczyce</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Jawczyce, Biskupice, wielicki, małopolskie</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>99000</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>99000</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H81" t="b">
+        <v>1</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>https://www.otodom.pl/pl/oferta/dzialka-budowlana-16-ar-jawczyce-ID4xr4L</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Działka budowlana | Koźmice Wielkie | gm. Wieliczka | 1416 m²</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Koźmice Wielkie, Wieliczka, wielicki, małopolskie</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>249000</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>249000</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H82" t="b">
+        <v>1</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>https://www.otodom.pl/pl/oferta/dzialka-budowlana-kozmice-wielkie-gm-wieliczka-1416-m-ID4xqLp</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>14a budowlane przy drodze z mediami, Krk Wieliczka</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Sygneczów, Wieliczka, wielicki, małopolskie</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>152500</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>152500</v>
+      </c>
+      <c r="G83" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H83" t="b">
+        <v>1</v>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>https://www.otodom.pl/pl/oferta/14a-budowlane-przy-drodze-z-mediami-krk-wieliczka-ID4xpge</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Kobylec | Działka budowlana przy Lesie -  ok. 14 ar / 179.000 zł</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Kobylec, Łapanów, bocheński, małopolskie</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>179000</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>179000</v>
+      </c>
+      <c r="G84" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H84" t="b">
+        <v>1</v>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>https://www.otodom.pl/pl/oferta/kobylec-dzialka-budowlana-przy-lesie-ok-14-ar-179-000-zl-ID4xjra</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Działka Budowlana | 16 ar | Jawczyce</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Jawczyce, Biskupice, wielicki, małopolskie</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>99000</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>99000</v>
+      </c>
+      <c r="G85" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H85" t="b">
+        <v>1</v>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>https://www.otodom.pl/hpr/pl/oferta/dzialka-budowlana-16-ar-jawczyce-ID4xr4L</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatic Excel update [2025-07-27 11:47:04]
</commit_message>
<xml_diff>
--- a/wyniki_ofert_z_filtra.xlsx
+++ b/wyniki_ofert_z_filtra.xlsx
@@ -1303,7 +1303,7 @@
         <v>0.49</v>
       </c>
       <c r="H22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -2785,7 +2785,7 @@
         <v>0.49</v>
       </c>
       <c r="H60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" t="inlineStr">
         <is>
@@ -2804,7 +2804,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4937,6 +4937,45 @@
         </is>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Atrakcyjna działka budowlana Grajów Wieliczka.</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Grajów, Wieliczka, wielicki, małopolskie</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>230000</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>2025-07-27</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>230000</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H55" t="b">
+        <v>1</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>https://www.otodom.pl/pl/oferta/atrakcyjna-dzialka-budowlana-grajow-wieliczka-ID4vwuO</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Automatic Excel update [2025-07-28 07:29:18]
</commit_message>
<xml_diff>
--- a/wyniki_ofert_z_filtra.xlsx
+++ b/wyniki_ofert_z_filtra.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -552,7 +552,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -591,7 +591,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -630,7 +630,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -669,7 +669,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -708,7 +708,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -747,7 +747,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -786,7 +786,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -825,7 +825,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -864,7 +864,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -903,7 +903,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -942,7 +942,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -981,7 +981,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -1020,7 +1020,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1098,7 +1098,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1215,7 +1215,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1332,7 +1332,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1410,7 +1410,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1527,7 +1527,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -1605,7 +1605,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1644,7 +1644,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -1722,7 +1722,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -1800,7 +1800,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -1839,7 +1839,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -1878,7 +1878,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -1917,7 +1917,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -1995,7 +1995,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -2034,7 +2034,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -2112,7 +2112,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -2190,7 +2190,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -2268,7 +2268,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -2307,7 +2307,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -2424,7 +2424,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -2463,7 +2463,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -2502,7 +2502,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F54" t="n">
@@ -2580,7 +2580,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -2619,7 +2619,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F56" t="n">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F57" t="n">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F58" t="n">
@@ -2736,7 +2736,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F59" t="n">
@@ -2891,7 +2891,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -2930,7 +2930,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -3008,7 +3008,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -3047,7 +3047,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -3086,7 +3086,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -3164,7 +3164,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -3203,7 +3203,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -3242,7 +3242,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -3320,7 +3320,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -3359,7 +3359,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -3437,7 +3437,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -3476,7 +3476,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -3515,7 +3515,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -3554,7 +3554,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -3593,7 +3593,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -3632,7 +3632,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -3671,7 +3671,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -3710,7 +3710,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -3749,7 +3749,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -3827,7 +3827,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -3905,7 +3905,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -3944,7 +3944,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -3983,7 +3983,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -4022,7 +4022,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -4061,7 +4061,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -4100,7 +4100,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -4139,7 +4139,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -4178,7 +4178,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -4217,7 +4217,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -4256,7 +4256,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -4295,7 +4295,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -4334,7 +4334,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -4373,7 +4373,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -4412,7 +4412,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -4451,7 +4451,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -4490,7 +4490,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -4529,7 +4529,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -4568,7 +4568,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -4607,7 +4607,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -4646,7 +4646,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -4685,7 +4685,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -4724,7 +4724,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -4763,7 +4763,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -4802,7 +4802,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -4841,7 +4841,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -4880,7 +4880,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -4958,7 +4958,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-07-28</t>
         </is>
       </c>
       <c r="F55" t="n">

</xml_diff>

<commit_message>
Automatic Excel update [2025-07-29 07:28:03]
</commit_message>
<xml_diff>
--- a/wyniki_ofert_z_filtra.xlsx
+++ b/wyniki_ofert_z_filtra.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,7 +513,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -552,7 +552,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -591,7 +591,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -630,7 +630,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -669,7 +669,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -708,7 +708,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -747,7 +747,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -786,7 +786,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -825,7 +825,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -864,7 +864,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -913,7 +913,7 @@
         <v>0.49</v>
       </c>
       <c r="H12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -942,7 +942,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -981,7 +981,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -1020,7 +1020,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1098,7 +1098,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1215,7 +1215,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1332,7 +1332,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1410,7 +1410,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1527,7 +1527,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -1605,7 +1605,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1644,7 +1644,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -1722,7 +1722,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -1800,7 +1800,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -1839,7 +1839,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -1878,7 +1878,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -1917,7 +1917,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -1995,7 +1995,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -2034,7 +2034,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -2112,7 +2112,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -2200,7 +2200,7 @@
         <v>0.49</v>
       </c>
       <c r="H45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -2268,7 +2268,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -2307,7 +2307,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -2424,7 +2424,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -2463,7 +2463,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -2502,7 +2502,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F54" t="n">
@@ -2580,7 +2580,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -2619,7 +2619,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F56" t="n">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F57" t="n">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F58" t="n">
@@ -2736,7 +2736,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F59" t="n">
@@ -2790,6 +2790,84 @@
       <c r="I60" t="inlineStr">
         <is>
           <t>https://www.otodom.pl/hpr/pl/oferta/14-ar-w-gm-liszki-ID4wlgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Działka blisko Krakowa w pięknej okolicy!</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Kamień, Czernichów, krakowski, małopolskie</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>248000</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2025-07-29</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2025-07-29</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>248000</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>https://www.otodom.pl/pl/oferta/dzialka-blisko-krakowa-w-pieknej-okolicy-ID4xcWR</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Mogilany - działka dla miłośników ogrodów. Polecam</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>ul. Górska, Mogilany, Mogilany, krakowski, małopolskie</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>250000</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2025-07-29</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>2025-07-29</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>250000</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H62" t="b">
+        <v>1</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>https://www.otodom.pl/pl/oferta/mogilany-dzialka-dla-milosnikow-ogrodow-polecam-ID4w22e</t>
         </is>
       </c>
     </row>
@@ -2804,7 +2882,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2891,7 +2969,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -2930,7 +3008,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -2969,7 +3047,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -3008,7 +3086,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -3047,7 +3125,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -3086,7 +3164,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -3125,7 +3203,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -3164,7 +3242,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -3203,7 +3281,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -3242,7 +3320,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -3281,7 +3359,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -3320,7 +3398,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -3359,7 +3437,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -3437,7 +3515,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -3486,7 +3564,7 @@
         <v>0.49</v>
       </c>
       <c r="H17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -3515,7 +3593,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -3554,7 +3632,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -3593,7 +3671,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -3632,7 +3710,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -3671,7 +3749,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -3710,7 +3788,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -3749,7 +3827,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -3788,7 +3866,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -3827,7 +3905,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -3866,7 +3944,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -3905,7 +3983,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -3944,7 +4022,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -3983,7 +4061,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -4022,7 +4100,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -4061,7 +4139,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -4100,7 +4178,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -4139,7 +4217,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -4178,7 +4256,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -4217,7 +4295,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -4256,7 +4334,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -4295,7 +4373,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -4334,7 +4412,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -4383,7 +4461,7 @@
         <v>0.49</v>
       </c>
       <c r="H40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
@@ -4412,7 +4490,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -4451,7 +4529,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -4490,7 +4568,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -4529,7 +4607,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -4568,7 +4646,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -4607,7 +4685,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -4646,7 +4724,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -4685,7 +4763,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -4724,7 +4802,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -4763,7 +4841,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -4802,7 +4880,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -4841,7 +4919,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -4880,7 +4958,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -4929,7 +5007,7 @@
         <v>0.49</v>
       </c>
       <c r="H54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" t="inlineStr">
         <is>
@@ -4958,7 +5036,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -4973,6 +5051,84 @@
       <c r="I55" t="inlineStr">
         <is>
           <t>https://www.otodom.pl/pl/oferta/atrakcyjna-dzialka-budowlana-grajow-wieliczka-ID4vwuO</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Działka budowlana 20a, koło Wieliczki</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Dobranowice, Wieliczka, wielicki, małopolskie</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>245000</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2025-07-29</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>2025-07-29</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>245000</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>https://www.otodom.pl/pl/oferta/dzialka-budowlana-20a-kolo-wieliczki-ID4xseG</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Działka budowlana 20a, koło Wieliczki</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Dobranowice, Wieliczka, wielicki, małopolskie</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>245000</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2025-07-29</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>2025-07-29</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>245000</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H57" t="b">
+        <v>1</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>https://www.otodom.pl/hpr/pl/oferta/dzialka-budowlana-20a-kolo-wieliczki-ID4xseG</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatic Excel update [2025-07-30 07:28:35]
</commit_message>
<xml_diff>
--- a/wyniki_ofert_z_filtra.xlsx
+++ b/wyniki_ofert_z_filtra.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,7 +513,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -552,7 +552,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -591,7 +591,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -630,7 +630,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -669,7 +669,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -708,7 +708,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -747,7 +747,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -786,7 +786,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -825,7 +825,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -864,7 +864,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -942,7 +942,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -991,7 +991,7 @@
         <v>0.49</v>
       </c>
       <c r="H14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1098,7 +1098,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1186,7 +1186,7 @@
         <v>0.49</v>
       </c>
       <c r="H19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1332,7 +1332,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1410,7 +1410,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1527,7 +1527,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -1605,7 +1605,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1644,7 +1644,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -1722,7 +1722,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -1800,7 +1800,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -1839,7 +1839,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -1878,7 +1878,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -1917,7 +1917,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -1995,7 +1995,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -2034,7 +2034,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -2112,7 +2112,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -2268,7 +2268,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -2307,7 +2307,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -2424,7 +2424,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -2463,7 +2463,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -2502,7 +2502,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F54" t="n">
@@ -2580,7 +2580,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -2619,7 +2619,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F56" t="n">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F57" t="n">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F58" t="n">
@@ -2736,7 +2736,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F59" t="n">
@@ -2814,7 +2814,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F61" t="n">
@@ -2853,7 +2853,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F62" t="n">
@@ -2868,6 +2868,123 @@
       <c r="I62" t="inlineStr">
         <is>
           <t>https://www.otodom.pl/pl/oferta/mogilany-dzialka-dla-milosnikow-ogrodow-polecam-ID4w22e</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Cała budowlana - tanio!! Cicha i spokojna okolica</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Igołomia, Igołomia-Wawrzeńczyce, krakowski, małopolskie</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>199000</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>199000</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H63" t="b">
+        <v>1</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>https://www.otodom.pl/pl/oferta/cala-budowlana-tanio-cicha-i-spokojna-okolica-ID4r26n</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Cicha, zielona, z dala od zgiełku</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Prandocin-Wysiołek, Słomniki, krakowski, małopolskie</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>179000</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>179000</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H64" t="b">
+        <v>1</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>https://www.otodom.pl/pl/oferta/cicha-zielona-z-dala-od-zgielku-ID4uPsJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Cała budowlana - tanio!! Cicha i spokojna okolica</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Igołomia, Igołomia-Wawrzeńczyce, krakowski, małopolskie</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>199000</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>199000</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H65" t="b">
+        <v>1</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>https://www.otodom.pl/hpr/pl/oferta/cala-budowlana-tanio-cicha-i-spokojna-okolica-ID4r26n</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2999,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2969,7 +3086,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -3008,7 +3125,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -3047,7 +3164,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -3086,7 +3203,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -3125,7 +3242,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -3164,7 +3281,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -3203,7 +3320,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -3242,7 +3359,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -3281,7 +3398,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -3320,7 +3437,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -3359,7 +3476,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -3398,7 +3515,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -3437,7 +3554,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -3515,7 +3632,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -3593,7 +3710,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -3632,7 +3749,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -3671,7 +3788,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -3720,7 +3837,7 @@
         <v>0.49</v>
       </c>
       <c r="H21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -3749,7 +3866,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -3788,7 +3905,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -3827,7 +3944,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -3866,7 +3983,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -3905,7 +4022,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -3944,7 +4061,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -3983,7 +4100,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -4022,7 +4139,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -4061,7 +4178,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -4100,7 +4217,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -4139,7 +4256,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -4178,7 +4295,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -4217,7 +4334,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -4256,7 +4373,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -4295,7 +4412,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -4334,7 +4451,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -4373,7 +4490,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -4412,7 +4529,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -4490,7 +4607,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -4529,7 +4646,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -4568,7 +4685,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -4607,7 +4724,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -4646,7 +4763,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -4685,7 +4802,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -4724,7 +4841,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -4763,7 +4880,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -4802,7 +4919,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -4841,7 +4958,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -4880,7 +4997,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -4919,7 +5036,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -4958,7 +5075,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -5036,7 +5153,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -5075,7 +5192,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-30</t>
         </is>
       </c>
       <c r="F56" t="n">
@@ -5124,11 +5241,128 @@
         <v>0.49</v>
       </c>
       <c r="H57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" t="inlineStr">
         <is>
           <t>https://www.otodom.pl/hpr/pl/oferta/dzialka-budowlana-20a-kolo-wieliczki-ID4xseG</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Cała budowlana - tanio!! Cicha i spokojna okolica</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Igołomia, Igołomia-Wawrzeńczyce, krakowski, małopolskie</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>199000</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>199000</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H58" t="b">
+        <v>1</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>https://www.otodom.pl/pl/oferta/cala-budowlana-tanio-cicha-i-spokojna-okolica-ID4r26n</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Działka budowlana Sygneczów gm. Wieliczka</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Sygneczów, Wieliczka, wielicki, małopolskie</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>152500</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>152500</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H59" t="b">
+        <v>1</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>https://www.otodom.pl/pl/oferta/dzialka-budowlana-sygneczow-gm-wieliczka-ID4xsHw</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Cała budowlana - tanio!! Cicha i spokojna okolica</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Igołomia, Igołomia-Wawrzeńczyce, krakowski, małopolskie</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>199000</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>199000</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H60" t="b">
+        <v>1</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>https://www.otodom.pl/hpr/pl/oferta/cala-budowlana-tanio-cicha-i-spokojna-okolica-ID4r26n</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatic Excel update [2025-07-31 07:27:43]
</commit_message>
<xml_diff>
--- a/wyniki_ofert_z_filtra.xlsx
+++ b/wyniki_ofert_z_filtra.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -552,7 +552,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -591,7 +591,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -630,7 +630,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -669,7 +669,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -708,7 +708,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -747,7 +747,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -786,7 +786,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -825,7 +825,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -864,7 +864,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -942,7 +942,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -1020,7 +1020,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1098,7 +1098,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1215,7 +1215,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1332,7 +1332,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1410,7 +1410,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1527,7 +1527,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -1605,7 +1605,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1644,7 +1644,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -1722,7 +1722,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -1800,7 +1800,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -1839,7 +1839,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -1878,7 +1878,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -1917,7 +1917,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -1995,7 +1995,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -2034,7 +2034,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -2112,7 +2112,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -2268,7 +2268,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -2307,7 +2307,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -2424,7 +2424,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -2463,7 +2463,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -2502,7 +2502,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F54" t="n">
@@ -2580,7 +2580,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -2619,7 +2619,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F56" t="n">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F57" t="n">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F58" t="n">
@@ -2736,7 +2736,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F59" t="n">
@@ -2814,7 +2814,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F61" t="n">
@@ -2853,7 +2853,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F62" t="n">
@@ -2892,7 +2892,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F63" t="n">
@@ -2931,7 +2931,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F64" t="n">
@@ -2980,7 +2980,7 @@
         <v>0.49</v>
       </c>
       <c r="H65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65" t="inlineStr">
         <is>
@@ -3086,7 +3086,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -3164,7 +3164,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -3203,7 +3203,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -3242,7 +3242,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -3320,7 +3320,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -3359,7 +3359,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -3398,7 +3398,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -3437,7 +3437,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -3476,7 +3476,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -3515,7 +3515,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -3554,7 +3554,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -3632,7 +3632,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -3710,7 +3710,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -3749,7 +3749,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -3798,7 +3798,7 @@
         <v>0.49</v>
       </c>
       <c r="H20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -3866,7 +3866,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -3905,7 +3905,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -3944,7 +3944,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -3983,7 +3983,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -4022,7 +4022,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -4061,7 +4061,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -4100,7 +4100,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -4139,7 +4139,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -4178,7 +4178,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -4217,7 +4217,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -4256,7 +4256,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -4295,7 +4295,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -4334,7 +4334,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -4373,7 +4373,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -4412,7 +4412,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -4451,7 +4451,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -4490,7 +4490,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -4529,7 +4529,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -4607,7 +4607,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -4646,7 +4646,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -4685,7 +4685,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -4724,7 +4724,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -4763,7 +4763,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -4802,7 +4802,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -4841,7 +4841,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -4880,7 +4880,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -4919,7 +4919,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -4958,7 +4958,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -4997,7 +4997,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -5036,7 +5036,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -5075,7 +5075,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -5153,7 +5153,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -5192,7 +5192,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F56" t="n">
@@ -5270,7 +5270,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F58" t="n">
@@ -5309,7 +5309,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="F59" t="n">
@@ -5358,7 +5358,7 @@
         <v>0.49</v>
       </c>
       <c r="H60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" t="inlineStr">
         <is>

</xml_diff>